<commit_message>
Co-authored-by: #MANI SENTHILNATHAN VIGNESH# <VIGNESH024@e.ntu.edu.sg>
</commit_message>
<xml_diff>
--- a/OOPproj2002/src/pkg_camp/user_passwords.xlsx
+++ b/OOPproj2002/src/pkg_camp/user_passwords.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1767" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -119,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B523"/>
+  <dimension ref="A1:B883"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4309,6 +4309,2886 @@
         <v>3</v>
       </c>
     </row>
+    <row r="524">
+      <c r="A524" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B524" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B525" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B526" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B527" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B528" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B529" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B530" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B531" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B532" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B533" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B534" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B535" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B536" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B537" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B538" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B539" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B540" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B541" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B542" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B543" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B544" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B545" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B546" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B547" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B548" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B549" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B550" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B551" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B552" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B553" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B554" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B555" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B556" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B557" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B558" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B559" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B560" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B561" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B562" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B563" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B564" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B565" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B566" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B567" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B568" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B569" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B570" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B571" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B572" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B573" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B574" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B575" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B576" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B577" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B578" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B579" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B580" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B581" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B582" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B583" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B584" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B585" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B586" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B587" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B588" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B589" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B590" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B591" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B592" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B593" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B594" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B595" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B596" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B597" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B598" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B599" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B600" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B601" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B602" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B603" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B604" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B605" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B606" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B607" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B608" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B609" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B610" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B611" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B612" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B613" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B614" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B615" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B616" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B617" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B618" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B619" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B620" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B621" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B622" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B623" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B624" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B625" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B626" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B627" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B628" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B629" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B630" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B631" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B632" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B633" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B634" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B635" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B636" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B637" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B638" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B639" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B640" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B641" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B642" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B643" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B644" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B645" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B646" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B647" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B648" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B649" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B650" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B651" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B652" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B653" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B654" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B655" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B656" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B657" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B658" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B659" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B660" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B661" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B662" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B663" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B664" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B665" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B666" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B667" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B668" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B669" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B670" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B671" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B672" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B673" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B674" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B675" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B676" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B677" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B678" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B679" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B680" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B681" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B682" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B683" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B684" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B685" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B686" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B687" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B688" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B689" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B690" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B691" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B692" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B693" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B694" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B695" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B696" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B697" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B698" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B699" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B700" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B701" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B702" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B703" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B704" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B705" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B706" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B707" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B708" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B709" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B710" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B711" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B712" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B713" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B714" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B715" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B716" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B717" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B718" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B719" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B720" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B721" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B722" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B723" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B724" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B725" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B726" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B727" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B728" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B729" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B730" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B731" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B732" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B733" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B734" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B735" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B736" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B737" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B738" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B739" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B740" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B741" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B742" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B743" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B744" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B745" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B746" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B747" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B748" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B749" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B750" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B751" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B752" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B753" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B754" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B755" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B756" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B757" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B758" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B759" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B760" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B761" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B762" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B763" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B764" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B765" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B766" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B767" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B768" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B769" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B770" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B771" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B772" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B773" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B774" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B775" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B776" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B777" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B778" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B779" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B780" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B781" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B782" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B783" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B784" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B785" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B786" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B787" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B788" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B789" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B790" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B791" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B792" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B793" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B794" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B795" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B796" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B797" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B798" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B799" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B800" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B801" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B802" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B803" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B804" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B805" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B806" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B807" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B808" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B809" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B810" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B811" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B812" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B813" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B814" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B815" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B816" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B817" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B818" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B819" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B820" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B821" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B822" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B823" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B824" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B825" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B826" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B827" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B828" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B829" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B830" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B831" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B832" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B833" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B834" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B835" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B836" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B837" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B838" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B839" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B840" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B841" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B842" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B843" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B844" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B845" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B846" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B847" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B848" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B849" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B850" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B851" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B852" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B853" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B854" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B855" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B856" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B857" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B858" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B859" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B860" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B861" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B862" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B863" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B864" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B865" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B866" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B867" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B868" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B869" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B870" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B871" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B872" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B873" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B874" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B875" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B876" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B877" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="B878" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="B879" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B880" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B881" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B882" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B883" t="s" s="0">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>